<commit_message>
add growth chamber progs for rest of exp
</commit_message>
<xml_diff>
--- a/growth_chamber_progs/TT25_field_climate_data_with_gc_dates.xlsx
+++ b/growth_chamber_progs/TT25_field_climate_data_with_gc_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2025_TT_psf/growth_chamber_progs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868B0813-D51C-F24A-80ED-CA1FBA2CB43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C293453C-8F50-0C47-B833-CA0DA13C237E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="4540" windowWidth="33320" windowHeight="17440" xr2:uid="{887B3705-8DFB-0C4D-A53D-2A5036E9BFD1}"/>
+    <workbookView xWindow="51380" yWindow="780" windowWidth="30540" windowHeight="18240" xr2:uid="{887B3705-8DFB-0C4D-A53D-2A5036E9BFD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>median_soilTemp_field</t>
   </si>
   <si>
-    <t>may16_may_31</t>
-  </si>
-  <si>
     <t>apr16_apr30</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>max_par</t>
+  </si>
+  <si>
+    <t>may16_may31</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:G3"/>
+      <selection activeCell="C5" sqref="C5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
         <v>7.7</v>
@@ -565,15 +565,15 @@
         <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>9.5</v>
@@ -596,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <v>12.5</v>
@@ -616,10 +616,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>14.5</v>
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>14.5</v>
@@ -662,10 +662,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>17.3</v>
@@ -688,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>18.100000000000001</v>
@@ -708,10 +708,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1">
         <v>18.100000000000001</v>
@@ -734,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1">
         <v>18.7</v>
@@ -754,10 +754,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1">
         <v>17.2</v>

</xml_diff>